<commit_message>
cleaned up stats and added data
</commit_message>
<xml_diff>
--- a/Data/nfl_historic_betting_data.xlsx
+++ b/Data/nfl_historic_betting_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinmcdonough/Documents/Fantasy_Project/daily_fantasy/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C706728-0829-C743-923B-89772DB2A0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13BD813-7788-C54A-90D7-26A7FE6511B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-260" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1911,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A803" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G828" sqref="G828"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>